<commit_message>
Update pathogens + cost per case
</commit_message>
<xml_diff>
--- a/Data/AttributionProportions.xlsx
+++ b/Data/AttributionProportions.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angus/Documents/AustralianFoodborneIllnessCosting/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\daughb\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C49F62D-737A-B346-B5BB-FBA6C4C94916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="520" windowWidth="19200" windowHeight="14200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Salmonella" sheetId="1" r:id="rId1"/>
     <sheet name="Gamma parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -148,7 +147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,17 +164,32 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -185,11 +199,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,29 +490,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -502,7 +523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +546,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -548,7 +569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -571,7 +592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -594,7 +615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -617,7 +638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -640,7 +661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -663,7 +684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -686,7 +707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -709,7 +730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -732,7 +753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -755,7 +776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -778,7 +799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -801,7 +822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -824,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -832,7 +853,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -840,7 +861,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -848,7 +869,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -856,7 +877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -884,7 +905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -898,7 +919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -912,7 +933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -926,7 +947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -940,7 +961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -954,7 +975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -968,7 +989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -982,7 +1003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
@@ -996,7 +1017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
@@ -1010,7 +1031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
@@ -1024,7 +1045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
@@ -1038,7 +1059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1052,12 +1073,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1069,19 +1090,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D131"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80:D131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1095,7 +1116,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1103,13 +1124,15 @@
         <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>14.299298</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>227.6361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1117,13 +1140,15 @@
         <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>18.866859999999999</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>1664.4839999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1131,13 +1156,15 @@
         <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>30.174465999999999</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>81.666849999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1145,13 +1172,15 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>18.918669999999999</v>
+        <v>18.91602</v>
       </c>
       <c r="D5" s="1">
-        <v>15504.075000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4613.201</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1159,13 +1188,15 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>9.4904550000000008</v>
+        <v>13.411830999999999</v>
       </c>
       <c r="D6" s="1">
-        <v>368.95830000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>182.00579999999999</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1173,13 +1204,15 @@
         <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>21.53004</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>1361.645</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1187,13 +1220,15 @@
         <v>10</v>
       </c>
       <c r="C8" s="1">
-        <v>12.413641</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>240.98510000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1201,13 +1236,15 @@
         <v>11</v>
       </c>
       <c r="C9" s="1">
-        <v>8.8554379999999995</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>206.53290000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1215,13 +1252,15 @@
         <v>12</v>
       </c>
       <c r="C10" s="1">
-        <v>12.280186</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>136.38760000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1229,13 +1268,15 @@
         <v>13</v>
       </c>
       <c r="C11" s="1">
-        <v>15.751671</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>64.772890000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1243,13 +1284,15 @@
         <v>14</v>
       </c>
       <c r="C12" s="1">
-        <v>14.38217</v>
+        <v>1746.3420799999999</v>
       </c>
       <c r="D12" s="1">
-        <v>4685.9439999999995</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2524.5210000000002</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1257,13 +1300,15 @@
         <v>15</v>
       </c>
       <c r="C13" s="1">
-        <v>32.015158999999997</v>
+        <v>20.493789</v>
       </c>
       <c r="D13" s="1">
-        <v>383.99349999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>149.81620000000001</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1271,13 +1316,15 @@
         <v>16</v>
       </c>
       <c r="C14" s="1">
-        <v>26.909220000000001</v>
+        <v>32.481001999999997</v>
       </c>
       <c r="D14" s="1">
-        <v>1528.674</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>442.15460000000002</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1291,7 +1338,7 @@
         <v>227.6361</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1305,7 +1352,7 @@
         <v>1664.4839999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1319,7 +1366,7 @@
         <v>81.666849999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1333,7 +1380,7 @@
         <v>15504.075000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1347,7 +1394,7 @@
         <v>368.95830000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1361,7 +1408,7 @@
         <v>1361.645</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1375,7 +1422,7 @@
         <v>240.98510000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1389,7 +1436,7 @@
         <v>206.53290000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1403,7 +1450,7 @@
         <v>136.38760000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1417,7 +1464,7 @@
         <v>64.772890000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1431,7 +1478,7 @@
         <v>4685.9439999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1445,7 +1492,7 @@
         <v>383.99349999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1459,245 +1506,265 @@
         <v>1528.674</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="1">
-        <v>14.299298</v>
-      </c>
-      <c r="D28" s="1">
-        <v>227.6361</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C28" s="5">
+        <v>2121.5926599999998</v>
+      </c>
+      <c r="D28" s="6">
+        <v>6140.5380000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="1">
-        <v>18.866859999999999</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1664.4839999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C29" s="5">
+        <v>195.20108999999999</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1299.0140000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="1">
-        <v>30.174465999999999</v>
-      </c>
-      <c r="D30" s="1">
-        <v>81.666849999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C30" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="D30" s="6">
+        <v>2262.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="1">
-        <v>18.918669999999999</v>
-      </c>
-      <c r="D31" s="1">
-        <v>15504.075000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C31" s="5">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="1">
-        <v>9.4904550000000008</v>
-      </c>
-      <c r="D32" s="1">
-        <v>368.95830000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="7">
+        <v>253.44914</v>
+      </c>
+      <c r="D32" s="8">
+        <v>6021.7160000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="1">
-        <v>21.53004</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1361.645</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="7">
+        <v>253.44914</v>
+      </c>
+      <c r="D33" s="8">
+        <v>6021.7160000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="1">
-        <v>12.413641</v>
-      </c>
-      <c r="D34" s="1">
-        <v>240.98510000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="5">
+        <v>672.23873000000003</v>
+      </c>
+      <c r="D34" s="6">
+        <v>9970.9959999999992</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="1">
-        <v>8.8554379999999995</v>
-      </c>
-      <c r="D35" s="1">
-        <v>206.53290000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="5">
+        <v>0</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>26</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="1">
-        <v>12.280186</v>
-      </c>
-      <c r="D36" s="1">
-        <v>136.38760000000002</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C36" s="5">
+        <v>3347.3090000000002</v>
+      </c>
+      <c r="D36" s="6">
+        <v>45149.599999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="1">
-        <v>15.751671</v>
-      </c>
-      <c r="D37" s="1">
-        <v>64.772890000000004</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C37" s="5">
+        <v>253.41893999999999</v>
+      </c>
+      <c r="D37" s="6">
+        <v>6021.0929999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>26</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="1">
-        <v>14.38217</v>
-      </c>
-      <c r="D38" s="1">
-        <v>4685.9439999999995</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>26</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="1">
-        <v>32.015158999999997</v>
-      </c>
-      <c r="D39" s="1">
-        <v>383.99349999999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C39" s="5">
+        <v>708.89349000000004</v>
+      </c>
+      <c r="D39" s="6">
+        <v>3587.3539999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="1">
-        <v>26.909220000000001</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1528.674</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>63.223390000000002</v>
+      </c>
+      <c r="D40">
+        <v>1596.6220000000001</v>
+      </c>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>28</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="1">
-        <v>14.299298</v>
-      </c>
-      <c r="D41" s="1">
-        <v>227.6361</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>6.9746459999999999</v>
+      </c>
+      <c r="D41">
+        <v>2675.1261</v>
+      </c>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>28</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="1">
-        <v>18.866859999999999</v>
-      </c>
-      <c r="D42" s="1">
-        <v>1664.4839999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>741.23163999999997</v>
+      </c>
+      <c r="D42">
+        <v>2151.297</v>
+      </c>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="1">
-        <v>30.174465999999999</v>
-      </c>
-      <c r="D43" s="1">
-        <v>81.666849999999997</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>28</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="1">
-        <v>18.918669999999999</v>
-      </c>
-      <c r="D44" s="1">
-        <v>15504.075000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>12.308579999999999</v>
+      </c>
+      <c r="D44">
+        <v>1607.8510000000001</v>
+      </c>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -1705,55 +1772,79 @@
         <v>8</v>
       </c>
       <c r="C45" s="1">
-        <v>9.4904550000000008</v>
+        <v>281.52803</v>
       </c>
       <c r="D45" s="1">
-        <v>368.95830000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1775.1290000000001</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="1">
-        <v>21.53004</v>
+      <c r="C46">
+        <v>24.87557</v>
       </c>
       <c r="D46" s="1">
-        <v>1361.645</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1028.538</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>10</v>
       </c>
-      <c r="C47" s="1">
-        <v>12.413641</v>
+      <c r="C47">
+        <v>6.8366610000000003</v>
       </c>
       <c r="D47" s="1">
-        <v>240.98510000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2618.9958000000001</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>28</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="1">
-        <v>8.8554379999999995</v>
+      <c r="C48">
+        <v>6.8366610000000003</v>
       </c>
       <c r="D48" s="1">
-        <v>206.53290000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2618.9958000000001</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -1761,1157 +1852,1223 @@
         <v>12</v>
       </c>
       <c r="C49" s="1">
-        <v>12.280186</v>
+        <v>3778.0810000000001</v>
       </c>
       <c r="D49" s="1">
-        <v>136.38760000000002</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>48978.400000000001</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>28</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="1">
-        <v>15.751671</v>
-      </c>
-      <c r="D50" s="1">
-        <v>64.772890000000004</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="10">
+        <v>3470.3215</v>
+      </c>
+      <c r="D50" s="10">
+        <v>46486.18</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>28</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="1">
-        <v>14.38217</v>
-      </c>
-      <c r="D51" s="1">
-        <v>4685.9439999999995</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C51" s="10">
+        <v>3470.3215</v>
+      </c>
+      <c r="D51" s="10">
+        <v>46486.18</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>28</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="1">
-        <v>32.015158999999997</v>
+      <c r="C52" s="9">
+        <v>761.36982999999998</v>
       </c>
       <c r="D52" s="1">
-        <v>383.99349999999998</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4025.998</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>28</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="1">
-        <v>26.909220000000001</v>
+      <c r="C53" s="3">
+        <v>16.152184999999999</v>
       </c>
       <c r="D53" s="1">
-        <v>1528.674</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>490.65719999999999</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>29</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C54" t="s">
-        <v>31</v>
-      </c>
-      <c r="D54" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>29</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C55" t="s">
-        <v>31</v>
-      </c>
-      <c r="D55" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>29</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C56" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>29</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C57" t="s">
-        <v>31</v>
-      </c>
-      <c r="D57" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C57" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>29</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C58" t="s">
-        <v>31</v>
-      </c>
-      <c r="D58" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>29</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C59" t="s">
-        <v>31</v>
-      </c>
-      <c r="D59" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>29</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C60" t="s">
-        <v>31</v>
-      </c>
-      <c r="D60" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>29</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C61" t="s">
-        <v>31</v>
-      </c>
-      <c r="D61" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>29</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C62" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>29</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D63" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C63" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>29</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C64" t="s">
-        <v>31</v>
-      </c>
-      <c r="D64" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C64" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>29</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C65" t="s">
-        <v>31</v>
-      </c>
-      <c r="D65" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C65" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>29</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C66" t="s">
-        <v>31</v>
-      </c>
-      <c r="D66" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C66" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>30</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C67" t="s">
-        <v>31</v>
-      </c>
-      <c r="D67" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C67" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>30</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C68" t="s">
-        <v>31</v>
-      </c>
-      <c r="D68" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C68" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>30</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C69" t="s">
-        <v>31</v>
-      </c>
-      <c r="D69" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C69" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>30</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C70" t="s">
-        <v>31</v>
-      </c>
-      <c r="D70" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C70" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>30</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C71" t="s">
-        <v>31</v>
-      </c>
-      <c r="D71" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C71" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>30</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C72" t="s">
-        <v>31</v>
-      </c>
-      <c r="D72" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C72" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>30</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C73" t="s">
-        <v>31</v>
-      </c>
-      <c r="D73" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C73" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>30</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C74" t="s">
-        <v>31</v>
-      </c>
-      <c r="D74" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C74" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>30</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C75" t="s">
-        <v>31</v>
-      </c>
-      <c r="D75" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C75" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>30</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C76" t="s">
-        <v>31</v>
-      </c>
-      <c r="D76" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C76" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>30</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C77" t="s">
-        <v>31</v>
-      </c>
-      <c r="D77" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C77" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>30</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C78" t="s">
-        <v>31</v>
-      </c>
-      <c r="D78" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C78" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>30</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C79" t="s">
-        <v>31</v>
-      </c>
-      <c r="D79" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C79" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>32</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C80" t="s">
-        <v>31</v>
-      </c>
-      <c r="D80" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C80" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>32</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C81" t="s">
-        <v>31</v>
-      </c>
-      <c r="D81" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C81" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>32</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C82" t="s">
-        <v>31</v>
-      </c>
-      <c r="D82" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C82" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>32</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C83" t="s">
-        <v>31</v>
-      </c>
-      <c r="D83" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C83" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>32</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C84" t="s">
-        <v>31</v>
-      </c>
-      <c r="D84" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C84" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>32</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C85" t="s">
-        <v>31</v>
-      </c>
-      <c r="D85" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C85" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>32</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C86" t="s">
-        <v>31</v>
-      </c>
-      <c r="D86" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C86" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>32</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C87" t="s">
-        <v>31</v>
-      </c>
-      <c r="D87" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C87" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>32</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C88" t="s">
-        <v>31</v>
-      </c>
-      <c r="D88" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>32</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C89" t="s">
-        <v>31</v>
-      </c>
-      <c r="D89" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C89" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>32</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C90" t="s">
-        <v>31</v>
-      </c>
-      <c r="D90" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C90" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>32</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C91" t="s">
-        <v>31</v>
-      </c>
-      <c r="D91" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C91" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>32</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C92" t="s">
-        <v>31</v>
-      </c>
-      <c r="D92" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C92" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>33</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C93" t="s">
-        <v>31</v>
-      </c>
-      <c r="D93" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C93" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>33</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C94" t="s">
-        <v>31</v>
-      </c>
-      <c r="D94" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C94" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>33</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C95" t="s">
-        <v>31</v>
-      </c>
-      <c r="D95" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C95" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>33</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C96" t="s">
-        <v>31</v>
-      </c>
-      <c r="D96" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C96" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>33</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C97" t="s">
-        <v>31</v>
-      </c>
-      <c r="D97" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C97" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>33</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C98" t="s">
-        <v>31</v>
-      </c>
-      <c r="D98" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C98" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>33</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C99" t="s">
-        <v>31</v>
-      </c>
-      <c r="D99" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C99" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>33</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C100" t="s">
-        <v>31</v>
-      </c>
-      <c r="D100" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C100" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>33</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C101" t="s">
-        <v>31</v>
-      </c>
-      <c r="D101" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C101" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>33</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C102" t="s">
-        <v>31</v>
-      </c>
-      <c r="D102" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C102" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>33</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C103" t="s">
-        <v>31</v>
-      </c>
-      <c r="D103" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C103" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>33</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C104" t="s">
-        <v>31</v>
-      </c>
-      <c r="D104" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C104" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>33</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C105" t="s">
-        <v>31</v>
-      </c>
-      <c r="D105" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C105" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>34</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C106" t="s">
-        <v>31</v>
-      </c>
-      <c r="D106" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C106" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>34</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C107" t="s">
-        <v>31</v>
-      </c>
-      <c r="D107" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C107" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>34</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C108" t="s">
-        <v>31</v>
-      </c>
-      <c r="D108" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C108" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>34</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C109" t="s">
-        <v>31</v>
-      </c>
-      <c r="D109" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C109" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>34</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C110" t="s">
-        <v>31</v>
-      </c>
-      <c r="D110" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C110" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>34</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C111" t="s">
-        <v>31</v>
-      </c>
-      <c r="D111" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C111" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>34</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C112" t="s">
-        <v>31</v>
-      </c>
-      <c r="D112" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C112" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>34</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C113" t="s">
-        <v>31</v>
-      </c>
-      <c r="D113" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C113" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>34</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C114" t="s">
-        <v>31</v>
-      </c>
-      <c r="D114" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C114" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>34</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C115" t="s">
-        <v>31</v>
-      </c>
-      <c r="D115" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C115" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>34</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C116" t="s">
-        <v>31</v>
-      </c>
-      <c r="D116" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C116" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>34</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C117" t="s">
-        <v>31</v>
-      </c>
-      <c r="D117" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C117" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>34</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C118" t="s">
-        <v>31</v>
-      </c>
-      <c r="D118" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C118" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>35</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C119" t="s">
-        <v>31</v>
-      </c>
-      <c r="D119" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C119" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>35</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C120" t="s">
-        <v>31</v>
-      </c>
-      <c r="D120" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C120" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C121" t="s">
-        <v>31</v>
-      </c>
-      <c r="D121" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C121" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>35</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C122" t="s">
-        <v>31</v>
-      </c>
-      <c r="D122" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C122" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>35</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C123" t="s">
-        <v>31</v>
-      </c>
-      <c r="D123" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C123" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>35</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C124" t="s">
-        <v>31</v>
-      </c>
-      <c r="D124" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C124" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>35</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C125" t="s">
-        <v>31</v>
-      </c>
-      <c r="D125" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C125" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>35</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C126" t="s">
-        <v>31</v>
-      </c>
-      <c r="D126" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C126" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>35</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C127" t="s">
-        <v>31</v>
-      </c>
-      <c r="D127" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C127" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>35</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C128" t="s">
-        <v>31</v>
-      </c>
-      <c r="D128" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C128" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>35</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C129" t="s">
-        <v>31</v>
-      </c>
-      <c r="D129" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C129" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>35</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C130" t="s">
-        <v>31</v>
-      </c>
-      <c r="D130" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C130" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>35</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C131" t="s">
-        <v>31</v>
-      </c>
-      <c r="D131" t="s">
+      <c r="C131" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2927,7 +3084,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09CFC866-F85E-4F76-8FB6-ECF461D9B56F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{943E2F57-2D43-4546-93BA-FD67B31B43B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>